<commit_message>
add cache in billing
</commit_message>
<xml_diff>
--- a/Billing/allResources.xlsx
+++ b/Billing/allResources.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Microsoft Azure Estimate</t>
   </si>
@@ -95,7 +95,7 @@
     <t>Internal Database</t>
   </si>
   <si>
-    <t xml:space="preserve">Single Database, vCore, General Purpose, Provisioned, Standard-series (Gen 5), Primary or Geo replica Disaster Recovery, Zone Redundant, 1 - 2 vCore Database(s) x 730 Hours, 300 GB Storage, SQL Licence (Pay as you go), ZRS Back up Storage Redundancy, 300 GB Point-In-Time Restore,  2 x 100 GB Long Term Retention</t>
+    <t xml:space="preserve">Single Database, vCore, General Purpose, Provisioned, Standard-series (Gen 5), Primary or Geo replica Disaster Recovery, Zone Redundant, 1 - 2 vCore Database(s) x 730 Hours, 300 GB Storage, SQL Licence (Pay as you go), ZRS Back up Storage Redundancy, 300 GB Point-In-Time Restore,  3 x 100 GB Long Term Retention</t>
   </si>
   <si>
     <t>Azure Functions</t>
@@ -206,6 +206,21 @@
     <t>Phone numbers leasing: 0 local and 0 toll-free United States (+1) phone number(s); Phone number lookup: 0 line type queries; Voice and Video Calling - over IP: 1 reoccurring call(s) (30 minutes X 0 call(s) per month X 0 participants per call); Call Recording: 0 Mixed audio recorded minutes, 0 Mixed audio and video recorded minutes, 0 Unmixed audio minutes for 0 participants; SIP Direct Routing: 0 Inbound calling minutes, 0 Outbound calling minutes; Chat: 0 chat users x 0 message(s) sent per chat user; Email: 21000 Email sent per month, 0.015 MB per Email; Whatsapp messaging: 0 Inbound messages, 0 Outbound messages; Job Router: 0 Jobs Routed per month</t>
   </si>
   <si>
+    <t>Azure Cache for Redis</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>Standard tier; 1 C3 instances x 730 Hours</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">Single Database, vCore, General Purpose, Provisioned, Standard-series (Gen 5), Primary or Geo replica Disaster Recovery, Zone Redundant, 1 - 2 vCore Database(s) x 730 Hours, 300 GB Storage, SQL Licence (Pay as you go), RA-GRS Back up Storage Redundancy, 300 GB Point-In-Time Restore,  3 x 100 GB Long Term Retention</t>
+  </si>
+  <si>
     <t>Support</t>
   </si>
   <si>
@@ -216,9 +231,6 @@
   </si>
   <si>
     <t>Billing Account</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Billing Profile</t>
@@ -233,7 +245,7 @@
     <t>All prices shown are in Euro Zone – Euro (€) EUR. This is a summary estimate, not a quote. For up to date pricing information please visit https://azure.microsoft.com/pricing/calculator/</t>
   </si>
   <si>
-    <t>This estimate was created at 7/24/2024 11:39:05 AM UTC.</t>
+    <t>This estimate was created at 7/24/2024 3:32:32 PM UTC.</t>
   </si>
 </sst>
 </file>
@@ -674,7 +686,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="5">
-        <v>693.314609371343</v>
+        <v>696.97514394045777</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -1241,16 +1253,22 @@
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="13" t="s">
-        <v>64</v>
+      <c r="C22" s="3" t="s">
+        <v>65</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="D22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="F22" s="5">
-        <v>93.619809951785783</v>
+        <v>384.08463230819638</v>
       </c>
       <c r="G22" s="5">
         <v>0</v>
@@ -1276,17 +1294,27 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="13" t="s">
-        <v>65</v>
+      <c r="A23" s="3" t="s">
+        <v>24</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>66</v>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="C23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="5">
+        <v>731.63319758460887</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
       <c r="H23" s="7"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1308,17 +1336,21 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24">
-      <c r="A24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>68</v>
+      <c r="E24" s="12"/>
+      <c r="F24" s="5">
+        <v>93.619809951785783</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
       <c r="H24" s="7"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1344,10 +1376,10 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -1375,16 +1407,14 @@
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="14" t="s">
-        <v>70</v>
+      <c r="D26" s="13" t="s">
+        <v>72</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="15">
-        <v>12601.893367036466</v>
+      <c r="E26" s="13" t="s">
+        <v>67</v>
       </c>
-      <c r="G26" s="15">
-        <v>0</v>
-      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
       <c r="H26" s="7"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1409,8 +1439,12 @@
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="7"/>
@@ -1434,15 +1468,19 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28">
-      <c r="A28" s="13" t="s">
-        <v>71</v>
-      </c>
+      <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="D28" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="15">
+        <v>13721.271731498386</v>
+      </c>
+      <c r="G28" s="15">
+        <v>0</v>
+      </c>
       <c r="H28" s="7"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1464,15 +1502,13 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29">
-      <c r="A29" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
       <c r="H29" s="7"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1494,15 +1530,15 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30">
-      <c r="A30" s="16" t="s">
-        <v>73</v>
+      <c r="A30" s="13" t="s">
+        <v>75</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
       <c r="H30" s="7"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1524,7 +1560,9 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31">
-      <c r="A31" s="16"/>
+      <c r="A31" s="16" t="s">
+        <v>76</v>
+      </c>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -1552,13 +1590,15 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="A32" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
       <c r="H32" s="7"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1580,13 +1620,13 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
       <c r="H33" s="7"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -28687,8 +28727,8 @@
   <mergeCells>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A32:G32"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>